<commit_message>
baseline and windspeed updates
</commit_message>
<xml_diff>
--- a/notebooks/oneday_terrain.xlsx
+++ b/notebooks/oneday_terrain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrmik\OneDrive\Desktop\NSS\Python\Projects\Cycling_Capstone\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C29F3-8434-4826-8164-5FDE338F06DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EED541-A1D6-428E-87FC-771285BE7380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-9240" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -840,13 +840,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="43.21875" customWidth="1"/>
     <col min="3" max="3" width="39.88671875" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
+    <col min="15" max="15" width="12.77734375" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" customWidth="1"/>
+    <col min="17" max="17" width="17.77734375" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" customWidth="1"/>
+    <col min="22" max="22" width="19.33203125" customWidth="1"/>
+    <col min="23" max="23" width="23.109375" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">

</xml_diff>